<commit_message>
Global refactoring of maplayer page
</commit_message>
<xml_diff>
--- a/public/data/persons.xlsx
+++ b/public/data/persons.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="1460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="1463">
   <si>
     <t>Источник</t>
   </si>
@@ -4095,9 +4095,6 @@
     <t>Будучи командиром полка сражался в осаждённом Могилёве. Смог выйти из окружения, за что был представлен к ордену Красного Знамени</t>
   </si>
   <si>
-    <t>31.11.1976</t>
-  </si>
-  <si>
     <t>Могилёв</t>
   </si>
   <si>
@@ -4461,6 +4458,18 @@
   </si>
   <si>
     <t>Сталинград; Донецк; Ростов-на-Дону</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/ru/c/ca/Генерал_И.Е.Петров._ТуркВО%2C_1931.jpg</t>
+  </si>
+  <si>
+    <t>Волгоград</t>
+  </si>
+  <si>
+    <t>Уфа</t>
+  </si>
+  <si>
+    <t>За умелое управление войсками при форсировании рек Десна, Днепр, Припять и проявленные при этом мужество и отвагу 16 октября 1943 года генерал-лейтенанту Пухову присвоено звание Героя Советского Союза</t>
   </si>
 </sst>
 </file>
@@ -4586,7 +4595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4697,9 +4706,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="17" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -4725,6 +4731,12 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5393,10 +5405,10 @@
   <dimension ref="A1:R525"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K20" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="J138" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
+      <selection pane="bottomRight" activeCell="I135" sqref="I135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5514,7 +5526,7 @@
         <v>873</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="O2" s="13" t="s">
         <v>663</v>
@@ -5561,7 +5573,7 @@
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="8" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="O3" s="8"/>
       <c r="P3" t="s">
@@ -5604,7 +5616,7 @@
       </c>
       <c r="M4" s="8"/>
       <c r="N4" s="8" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="O4" s="8"/>
       <c r="P4" s="6"/>
@@ -6048,7 +6060,7 @@
       <c r="Q14"/>
       <c r="R14" s="34"/>
     </row>
-    <row r="15" spans="1:18" ht="131.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8" t="s">
         <v>394</v>
@@ -6085,7 +6097,7 @@
         <v>850</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="O15" s="13"/>
       <c r="P15" s="6" t="s">
@@ -6129,7 +6141,7 @@
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="8" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="O16" s="13"/>
       <c r="P16" t="s">
@@ -6177,7 +6189,7 @@
       <c r="N17" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="O17" s="47" t="s">
+      <c r="O17" s="46" t="s">
         <v>662</v>
       </c>
       <c r="P17" s="6"/>
@@ -6220,7 +6232,7 @@
         <v>852</v>
       </c>
       <c r="N18" s="8"/>
-      <c r="O18" s="53"/>
+      <c r="O18" s="52"/>
       <c r="P18" s="6"/>
       <c r="R18" s="6"/>
     </row>
@@ -6261,7 +6273,7 @@
       <c r="N19" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="O19" s="53"/>
+      <c r="O19" s="52"/>
       <c r="P19" t="s">
         <v>308</v>
       </c>
@@ -6303,7 +6315,7 @@
         <v>859</v>
       </c>
       <c r="N20" s="30" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="O20" s="13" t="s">
         <v>661</v>
@@ -6386,7 +6398,7 @@
       </c>
       <c r="M22" s="7"/>
       <c r="N22" s="30" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="O22" s="13"/>
       <c r="P22" t="s">
@@ -6467,17 +6479,17 @@
       <c r="J24" s="8" t="s">
         <v>1111</v>
       </c>
-      <c r="K24" s="48">
+      <c r="K24" s="47">
         <v>15906</v>
       </c>
       <c r="L24" s="29" t="s">
         <v>867</v>
       </c>
-      <c r="M24" s="49"/>
+      <c r="M24" s="48"/>
       <c r="N24" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="O24" s="47" t="s">
+      <c r="O24" s="46" t="s">
         <v>692</v>
       </c>
       <c r="P24" t="s">
@@ -6511,7 +6523,7 @@
       <c r="J25" s="8" t="s">
         <v>715</v>
       </c>
-      <c r="K25" s="50" t="s">
+      <c r="K25" s="49" t="s">
         <v>868</v>
       </c>
       <c r="L25" s="29" t="s">
@@ -6767,10 +6779,10 @@
         <v>741</v>
       </c>
       <c r="K31" s="9">
-        <v>15276</v>
+        <v>32037</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>14</v>
+        <v>1461</v>
       </c>
       <c r="M31" s="8" t="s">
         <v>856</v>
@@ -6824,7 +6836,7 @@
       <c r="N32" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="O32" s="47" t="s">
+      <c r="O32" s="46" t="s">
         <v>324</v>
       </c>
       <c r="R32"/>
@@ -6911,7 +6923,7 @@
         <v>14</v>
       </c>
       <c r="M34" s="7"/>
-      <c r="N34" s="51"/>
+      <c r="N34" s="50"/>
       <c r="O34" s="8"/>
       <c r="R34"/>
     </row>
@@ -7304,7 +7316,7 @@
       </c>
       <c r="L44" s="11"/>
       <c r="M44" s="7"/>
-      <c r="N44" s="46"/>
+      <c r="N44" s="45"/>
       <c r="O44" s="15" t="s">
         <v>913</v>
       </c>
@@ -7334,10 +7346,10 @@
         <v>241</v>
       </c>
       <c r="I45" s="8" t="s">
+        <v>1340</v>
+      </c>
+      <c r="J45" s="8" t="s">
         <v>1341</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>1342</v>
       </c>
       <c r="K45" s="19" t="s">
         <v>914</v>
@@ -7787,7 +7799,9 @@
       <c r="K56" s="7" t="s">
         <v>1089</v>
       </c>
-      <c r="L56" s="8"/>
+      <c r="L56" s="8" t="s">
+        <v>1460</v>
+      </c>
       <c r="M56" s="7"/>
       <c r="N56" s="8"/>
       <c r="O56" s="8"/>
@@ -8021,10 +8035,10 @@
         <v>259</v>
       </c>
       <c r="I62" s="8" t="s">
+        <v>1343</v>
+      </c>
+      <c r="J62" s="8" t="s">
         <v>1344</v>
-      </c>
-      <c r="J62" s="8" t="s">
-        <v>1345</v>
       </c>
       <c r="K62" s="8" t="s">
         <v>1091</v>
@@ -8065,10 +8079,10 @@
         <v>128</v>
       </c>
       <c r="I63" s="8" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J63" s="8" t="s">
         <v>1346</v>
-      </c>
-      <c r="J63" s="8" t="s">
-        <v>1347</v>
       </c>
       <c r="K63" s="10">
         <v>28165</v>
@@ -8333,7 +8347,7 @@
         <v>889</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="J70" s="15" t="s">
         <v>134</v>
@@ -8415,7 +8429,7 @@
         <v>958</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="J72" s="8" t="s">
         <v>957</v>
@@ -8452,7 +8466,7 @@
       </c>
       <c r="H73" s="8"/>
       <c r="I73" s="8" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="J73" s="8" t="s">
         <v>583</v>
@@ -8489,10 +8503,10 @@
         <v>174</v>
       </c>
       <c r="I74" s="8" t="s">
+        <v>1348</v>
+      </c>
+      <c r="J74" s="8" t="s">
         <v>1349</v>
-      </c>
-      <c r="J74" s="8" t="s">
-        <v>1350</v>
       </c>
       <c r="K74" s="10">
         <v>16320</v>
@@ -8570,7 +8584,7 @@
         <v>220</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="K76" s="9">
         <v>16015</v>
@@ -8607,7 +8621,7 @@
       </c>
       <c r="H77" s="8"/>
       <c r="I77" s="8" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="J77" s="8" t="s">
         <v>631</v>
@@ -8725,7 +8739,7 @@
         <v>391</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="J80" s="8" t="s">
         <v>944</v>
@@ -9045,7 +9059,7 @@
         <v>1152</v>
       </c>
       <c r="K88" s="7" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="M88" s="7"/>
       <c r="O88" s="15" t="s">
@@ -9078,7 +9092,7 @@
         <v>391</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="J89" s="8" t="s">
         <v>948</v>
@@ -9114,17 +9128,17 @@
         <v>479</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="J90" s="8" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="K90" s="10">
         <v>15386</v>
       </c>
       <c r="M90" s="7"/>
       <c r="O90" s="8" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="P90"/>
       <c r="Q90" s="6"/>
@@ -9153,7 +9167,7 @@
         <v>391</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="J91" s="8" t="s">
         <v>949</v>
@@ -9186,7 +9200,7 @@
         <v>902</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="J92" s="8" t="s">
         <v>649</v>
@@ -9300,7 +9314,7 @@
         <v>951</v>
       </c>
       <c r="J95" s="8" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="K95" s="18">
         <v>37901</v>
@@ -9380,12 +9394,12 @@
         <v>118</v>
       </c>
       <c r="I97" s="39" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="J97" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="K97" s="54">
+      <c r="K97" s="53">
         <v>14912</v>
       </c>
       <c r="L97" s="39"/>
@@ -9421,7 +9435,7 @@
         <v>391</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="J98" s="8" t="s">
         <v>950</v>
@@ -9455,7 +9469,7 @@
         <v>901</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="J99" s="8" t="s">
         <v>925</v>
@@ -9491,7 +9505,7 @@
         <v>391</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="J100" s="8" t="s">
         <v>952</v>
@@ -9532,10 +9546,10 @@
         <v>163</v>
       </c>
       <c r="I101" s="8" t="s">
+        <v>1360</v>
+      </c>
+      <c r="J101" s="8" t="s">
         <v>1361</v>
-      </c>
-      <c r="J101" s="8" t="s">
-        <v>1362</v>
       </c>
       <c r="K101" s="10">
         <v>18168</v>
@@ -9606,7 +9620,7 @@
         <v>1263</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J103" s="8" t="s">
         <v>945</v>
@@ -9643,7 +9657,7 @@
         <v>1155</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="J104" s="8" t="s">
         <v>1154</v>
@@ -9682,10 +9696,10 @@
         <v>478</v>
       </c>
       <c r="I105" s="8" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J105" s="9" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="K105" s="9">
         <v>23340</v>
@@ -9720,7 +9734,7 @@
         <v>391</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="J106" s="8" t="s">
         <v>953</v>
@@ -9755,7 +9769,7 @@
         <v>391</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="J107" s="8" t="s">
         <v>954</v>
@@ -9791,7 +9805,7 @@
         <v>900</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="J108" s="8" t="s">
         <v>907</v>
@@ -9983,7 +9997,7 @@
         <v>391</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="J113" s="8" t="s">
         <v>590</v>
@@ -10060,7 +10074,7 @@
         <v>191</v>
       </c>
       <c r="J115" s="8" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="K115" s="7">
         <v>1981</v>
@@ -10096,10 +10110,10 @@
         <v>970</v>
       </c>
       <c r="I116" s="8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="J116" s="8" t="s">
         <v>1399</v>
-      </c>
-      <c r="J116" s="8" t="s">
-        <v>1400</v>
       </c>
       <c r="K116" s="9">
         <v>33435</v>
@@ -10364,10 +10378,10 @@
         <v>983</v>
       </c>
       <c r="I122" s="8" t="s">
+        <v>1362</v>
+      </c>
+      <c r="J122" s="8" t="s">
         <v>1363</v>
-      </c>
-      <c r="J122" s="8" t="s">
-        <v>1364</v>
       </c>
       <c r="K122" s="9">
         <v>37726</v>
@@ -10428,14 +10442,14 @@
       <c r="R123"/>
     </row>
     <row r="124" spans="1:18" s="8" customFormat="1" ht="93.75" x14ac:dyDescent="0.3">
-      <c r="A124" s="38"/>
+      <c r="A124" s="39"/>
       <c r="B124" s="39" t="s">
         <v>560</v>
       </c>
-      <c r="C124" s="38" t="s">
+      <c r="C124" s="39" t="s">
         <v>545</v>
       </c>
-      <c r="D124" s="38" t="s">
+      <c r="D124" s="39" t="s">
         <v>524</v>
       </c>
       <c r="E124" s="43" t="s">
@@ -10452,20 +10466,20 @@
         <v>1125</v>
       </c>
       <c r="J124" s="39" t="s">
-        <v>935</v>
-      </c>
-      <c r="K124" s="44">
+        <v>1459</v>
+      </c>
+      <c r="K124" s="55">
         <v>21282</v>
       </c>
       <c r="L124" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="M124" s="38"/>
+      <c r="M124" s="39"/>
       <c r="N124" s="39"/>
       <c r="O124" s="39"/>
-      <c r="P124" s="41"/>
-      <c r="Q124" s="41"/>
-      <c r="R124" s="41"/>
+      <c r="P124" s="56"/>
+      <c r="Q124" s="56"/>
+      <c r="R124" s="56"/>
     </row>
     <row r="125" spans="1:18" s="8" customFormat="1" ht="187.5" x14ac:dyDescent="0.3">
       <c r="B125" s="8" t="s">
@@ -10536,7 +10550,7 @@
         <v>995</v>
       </c>
       <c r="I126" s="8" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="J126" s="9" t="s">
         <v>1105</v>
@@ -10638,7 +10652,7 @@
         <v>31364</v>
       </c>
       <c r="M128" s="7"/>
-      <c r="N128" s="51"/>
+      <c r="N128" s="50"/>
       <c r="O128" s="15" t="s">
         <v>722</v>
       </c>
@@ -10715,10 +10729,10 @@
         <v>1013</v>
       </c>
       <c r="I130" s="8" t="s">
+        <v>1365</v>
+      </c>
+      <c r="J130" s="8" t="s">
         <v>1366</v>
-      </c>
-      <c r="J130" s="8" t="s">
-        <v>1367</v>
       </c>
       <c r="K130" s="9">
         <v>40215</v>
@@ -10759,7 +10773,7 @@
         <v>936</v>
       </c>
       <c r="I131" s="8" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="J131" s="8" t="s">
         <v>651</v>
@@ -10793,7 +10807,7 @@
         <v>932</v>
       </c>
       <c r="I132" s="8" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="J132" s="8" t="s">
         <v>587</v>
@@ -10818,7 +10832,7 @@
         <v>223</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="E133" s="9">
         <v>9548</v>
@@ -10872,10 +10886,10 @@
         <v>1016</v>
       </c>
       <c r="I134" s="8" t="s">
+        <v>1367</v>
+      </c>
+      <c r="J134" s="8" t="s">
         <v>1368</v>
-      </c>
-      <c r="J134" s="8" t="s">
-        <v>1369</v>
       </c>
       <c r="K134" s="9">
         <v>37403</v>
@@ -10915,6 +10929,9 @@
       <c r="G135" s="15" t="s">
         <v>909</v>
       </c>
+      <c r="H135" s="8" t="s">
+        <v>1462</v>
+      </c>
       <c r="I135" s="8" t="s">
         <v>929</v>
       </c>
@@ -10952,10 +10969,10 @@
         <v>1020</v>
       </c>
       <c r="I136" s="8" t="s">
+        <v>1369</v>
+      </c>
+      <c r="J136" s="8" t="s">
         <v>1370</v>
-      </c>
-      <c r="J136" s="8" t="s">
-        <v>1371</v>
       </c>
       <c r="K136" s="9">
         <v>35427</v>
@@ -10986,7 +11003,7 @@
       <c r="D137" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="E137" s="52">
+      <c r="E137" s="51">
         <v>3327</v>
       </c>
       <c r="F137" s="33" t="s">
@@ -10999,18 +11016,18 @@
         <v>1020</v>
       </c>
       <c r="I137" s="33" t="s">
+        <v>1369</v>
+      </c>
+      <c r="J137" s="51" t="s">
         <v>1370</v>
       </c>
-      <c r="J137" s="52" t="s">
-        <v>1371</v>
-      </c>
-      <c r="K137" s="52">
+      <c r="K137" s="51">
         <v>35427</v>
       </c>
       <c r="L137" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="M137" s="52">
+      <c r="M137" s="51">
         <v>16275</v>
       </c>
       <c r="N137" s="33" t="s">
@@ -11051,7 +11068,7 @@
         <v>1265</v>
       </c>
       <c r="J138" s="8" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="K138" s="9">
         <v>33229</v>
@@ -11145,6 +11162,9 @@
       <c r="K140" s="10">
         <v>25053</v>
       </c>
+      <c r="L140" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="M140" s="7"/>
       <c r="P140"/>
     </row>
@@ -11203,10 +11223,10 @@
         <v>1035</v>
       </c>
       <c r="I142" s="8" t="s">
+        <v>1371</v>
+      </c>
+      <c r="J142" s="8" t="s">
         <v>1372</v>
-      </c>
-      <c r="J142" s="8" t="s">
-        <v>1373</v>
       </c>
       <c r="K142" s="9">
         <v>33817</v>
@@ -11262,7 +11282,7 @@
       <c r="M143" s="42">
         <v>15894</v>
       </c>
-      <c r="N143" s="55" t="s">
+      <c r="N143" s="54" t="s">
         <v>1040</v>
       </c>
       <c r="O143" s="39" t="s">
@@ -11297,10 +11317,10 @@
         <v>1044</v>
       </c>
       <c r="I144" s="8" t="s">
+        <v>1373</v>
+      </c>
+      <c r="J144" s="9" t="s">
         <v>1374</v>
-      </c>
-      <c r="J144" s="9" t="s">
-        <v>1375</v>
       </c>
       <c r="K144" s="9">
         <v>32969</v>
@@ -11421,7 +11441,7 @@
         <v>930</v>
       </c>
       <c r="I147" s="8" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="J147" s="8" t="s">
         <v>642</v>
@@ -11486,7 +11506,7 @@
       <c r="D149" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="E149" s="52">
+      <c r="E149" s="51">
         <v>7959</v>
       </c>
       <c r="F149" s="33" t="s">
@@ -11499,18 +11519,18 @@
         <v>1170</v>
       </c>
       <c r="I149" s="33" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="J149" s="33" t="s">
-        <v>1379</v>
-      </c>
-      <c r="K149" s="52">
+        <v>1378</v>
+      </c>
+      <c r="K149" s="51">
         <v>30838</v>
       </c>
       <c r="L149" s="33" t="s">
         <v>1171</v>
       </c>
-      <c r="M149" s="45">
+      <c r="M149" s="44">
         <v>15676</v>
       </c>
       <c r="N149" s="39" t="s">
@@ -11536,7 +11556,7 @@
       <c r="D150" s="33" t="s">
         <v>1175</v>
       </c>
-      <c r="E150" s="52">
+      <c r="E150" s="51">
         <v>7712</v>
       </c>
       <c r="F150" s="33" t="s">
@@ -11549,18 +11569,18 @@
         <v>1177</v>
       </c>
       <c r="I150" s="33" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="J150" s="33" t="s">
-        <v>1380</v>
-      </c>
-      <c r="K150" s="52">
+        <v>1379</v>
+      </c>
+      <c r="K150" s="51">
         <v>40137</v>
       </c>
       <c r="L150" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M150" s="45">
+      <c r="M150" s="44">
         <v>15950</v>
       </c>
       <c r="N150" s="39" t="s">
@@ -11586,7 +11606,7 @@
       <c r="D151" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="E151" s="52">
+      <c r="E151" s="51">
         <v>7445</v>
       </c>
       <c r="F151" s="33" t="s">
@@ -11599,12 +11619,12 @@
         <v>1182</v>
       </c>
       <c r="I151" s="33" t="s">
+        <v>1380</v>
+      </c>
+      <c r="J151" s="33" t="s">
         <v>1381</v>
       </c>
-      <c r="J151" s="33" t="s">
-        <v>1382</v>
-      </c>
-      <c r="K151" s="52">
+      <c r="K151" s="51">
         <v>34621</v>
       </c>
       <c r="L151" s="33" t="s">
@@ -11672,7 +11692,7 @@
     <row r="153" spans="1:18" s="8" customFormat="1" ht="318.75" x14ac:dyDescent="0.3">
       <c r="A153" s="39"/>
       <c r="B153" s="39" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="C153" s="39" t="s">
         <v>1071</v>
@@ -11704,7 +11724,7 @@
       <c r="L153" s="39" t="s">
         <v>860</v>
       </c>
-      <c r="M153" s="45">
+      <c r="M153" s="44">
         <v>16254</v>
       </c>
       <c r="N153" s="39" t="s">
@@ -11728,7 +11748,7 @@
       <c r="D154" s="33" t="s">
         <v>533</v>
       </c>
-      <c r="E154" s="52">
+      <c r="E154" s="51">
         <v>6235</v>
       </c>
       <c r="F154" s="33" t="s">
@@ -11741,12 +11761,12 @@
         <v>1190</v>
       </c>
       <c r="I154" s="33" t="s">
+        <v>1382</v>
+      </c>
+      <c r="J154" s="33" t="s">
         <v>1383</v>
       </c>
-      <c r="J154" s="33" t="s">
-        <v>1384</v>
-      </c>
-      <c r="K154" s="52">
+      <c r="K154" s="51">
         <v>31996</v>
       </c>
       <c r="L154" s="33" t="s">
@@ -11778,7 +11798,7 @@
       <c r="D155" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="E155" s="52">
+      <c r="E155" s="51">
         <v>822</v>
       </c>
       <c r="F155" s="33" t="s">
@@ -11791,12 +11811,12 @@
         <v>1197</v>
       </c>
       <c r="I155" s="33" t="s">
+        <v>1384</v>
+      </c>
+      <c r="J155" s="33" t="s">
         <v>1385</v>
       </c>
-      <c r="J155" s="33" t="s">
-        <v>1386</v>
-      </c>
-      <c r="K155" s="52">
+      <c r="K155" s="51">
         <v>15155</v>
       </c>
       <c r="L155" s="33" t="s">
@@ -11837,13 +11857,16 @@
         <v>152</v>
       </c>
       <c r="I156" s="8" t="s">
+        <v>1386</v>
+      </c>
+      <c r="J156" s="8" t="s">
         <v>1387</v>
-      </c>
-      <c r="J156" s="8" t="s">
-        <v>1388</v>
       </c>
       <c r="K156" s="10">
         <v>36848</v>
+      </c>
+      <c r="L156" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="M156" s="7"/>
       <c r="N156" s="30"/>
@@ -11863,7 +11886,7 @@
       <c r="D157" s="33" t="s">
         <v>399</v>
       </c>
-      <c r="E157" s="52">
+      <c r="E157" s="51">
         <v>7409</v>
       </c>
       <c r="F157" s="33" t="s">
@@ -11876,12 +11899,12 @@
         <v>1203</v>
       </c>
       <c r="I157" s="33" t="s">
+        <v>1388</v>
+      </c>
+      <c r="J157" s="33" t="s">
         <v>1389</v>
       </c>
-      <c r="J157" s="33" t="s">
-        <v>1390</v>
-      </c>
-      <c r="K157" s="52">
+      <c r="K157" s="51">
         <v>39233</v>
       </c>
       <c r="L157" s="39" t="s">
@@ -11913,7 +11936,7 @@
       <c r="D158" s="33" t="s">
         <v>562</v>
       </c>
-      <c r="E158" s="52">
+      <c r="E158" s="51">
         <v>6516</v>
       </c>
       <c r="F158" s="33" t="s">
@@ -11926,18 +11949,18 @@
         <v>1209</v>
       </c>
       <c r="I158" s="33" t="s">
+        <v>1390</v>
+      </c>
+      <c r="J158" s="33" t="s">
         <v>1391</v>
       </c>
-      <c r="J158" s="33" t="s">
-        <v>1392</v>
-      </c>
-      <c r="K158" s="52">
+      <c r="K158" s="51">
         <v>17053</v>
       </c>
       <c r="L158" s="39" t="s">
         <v>1210</v>
       </c>
-      <c r="M158" s="45">
+      <c r="M158" s="44">
         <v>16011</v>
       </c>
       <c r="N158" s="39" t="s">
@@ -11963,7 +11986,7 @@
       <c r="D159" s="33" t="s">
         <v>428</v>
       </c>
-      <c r="E159" s="52">
+      <c r="E159" s="51">
         <v>4836</v>
       </c>
       <c r="F159" s="33" t="s">
@@ -11976,18 +11999,18 @@
         <v>1216</v>
       </c>
       <c r="I159" s="33" t="s">
+        <v>1403</v>
+      </c>
+      <c r="J159" s="33" t="s">
         <v>1404</v>
       </c>
-      <c r="J159" s="33" t="s">
-        <v>1405</v>
-      </c>
-      <c r="K159" s="52">
+      <c r="K159" s="51">
         <v>16420</v>
       </c>
       <c r="L159" s="33" t="s">
         <v>1217</v>
       </c>
-      <c r="M159" s="52">
+      <c r="M159" s="51">
         <v>16178</v>
       </c>
       <c r="N159" s="33" t="s">
@@ -12013,7 +12036,7 @@
       <c r="D160" s="33" t="s">
         <v>428</v>
       </c>
-      <c r="E160" s="52">
+      <c r="E160" s="51">
         <v>8178</v>
       </c>
       <c r="F160" s="33" t="s">
@@ -12026,18 +12049,18 @@
         <v>1222</v>
       </c>
       <c r="I160" s="33" t="s">
+        <v>1437</v>
+      </c>
+      <c r="J160" s="51" t="s">
         <v>1438</v>
       </c>
-      <c r="J160" s="52" t="s">
-        <v>1439</v>
-      </c>
-      <c r="K160" s="52">
+      <c r="K160" s="51">
         <v>34023</v>
       </c>
       <c r="L160" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M160" s="45">
+      <c r="M160" s="44">
         <v>16285</v>
       </c>
       <c r="N160" s="39" t="s">
@@ -12063,7 +12086,7 @@
       <c r="D161" s="33" t="s">
         <v>597</v>
       </c>
-      <c r="E161" s="52">
+      <c r="E161" s="51">
         <v>2758</v>
       </c>
       <c r="F161" s="33" t="s">
@@ -12076,18 +12099,18 @@
         <v>1228</v>
       </c>
       <c r="I161" s="33" t="s">
+        <v>1401</v>
+      </c>
+      <c r="J161" s="33" t="s">
         <v>1402</v>
       </c>
-      <c r="J161" s="33" t="s">
-        <v>1403</v>
-      </c>
-      <c r="K161" s="52">
+      <c r="K161" s="51">
         <v>15161</v>
       </c>
       <c r="L161" s="33" t="s">
         <v>1229</v>
       </c>
-      <c r="M161" s="52">
+      <c r="M161" s="51">
         <v>15161</v>
       </c>
       <c r="N161" s="33" t="s">
@@ -12127,7 +12150,7 @@
         <v>215</v>
       </c>
       <c r="J162" s="8" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="K162" s="19" t="s">
         <v>864</v>
@@ -12152,7 +12175,7 @@
       <c r="D163" s="33" t="s">
         <v>554</v>
       </c>
-      <c r="E163" s="52">
+      <c r="E163" s="51">
         <v>6123</v>
       </c>
       <c r="F163" s="33" t="s">
@@ -12165,18 +12188,18 @@
         <v>1234</v>
       </c>
       <c r="I163" s="33" t="s">
+        <v>1434</v>
+      </c>
+      <c r="J163" s="33" t="s">
         <v>1435</v>
       </c>
-      <c r="J163" s="33" t="s">
-        <v>1436</v>
-      </c>
-      <c r="K163" s="52">
+      <c r="K163" s="51">
         <v>38609</v>
       </c>
       <c r="L163" s="33" t="s">
         <v>1235</v>
       </c>
-      <c r="M163" s="45">
+      <c r="M163" s="44">
         <v>15858</v>
       </c>
       <c r="N163" s="39" t="s">
@@ -12220,13 +12243,13 @@
       <c r="J164" s="33" t="s">
         <v>1258</v>
       </c>
-      <c r="K164" s="52">
+      <c r="K164" s="51">
         <v>25658</v>
       </c>
       <c r="L164" s="33" t="s">
         <v>1243</v>
       </c>
-      <c r="M164" s="45">
+      <c r="M164" s="44">
         <v>15462</v>
       </c>
       <c r="N164" s="39" t="s">
@@ -12241,7 +12264,7 @@
     </row>
     <row r="165" spans="1:18" s="8" customFormat="1" ht="168.75" x14ac:dyDescent="0.3">
       <c r="B165" s="8" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="C165" s="8" t="s">
         <v>183</v>
@@ -12262,10 +12285,10 @@
         <v>1269</v>
       </c>
       <c r="I165" s="8" t="s">
+        <v>1432</v>
+      </c>
+      <c r="J165" s="9" t="s">
         <v>1433</v>
-      </c>
-      <c r="J165" s="9" t="s">
-        <v>1434</v>
       </c>
       <c r="K165" s="9">
         <v>32760</v>
@@ -12290,7 +12313,7 @@
     </row>
     <row r="166" spans="1:18" s="8" customFormat="1" ht="225" x14ac:dyDescent="0.3">
       <c r="B166" s="8" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="C166" s="8" t="s">
         <v>509</v>
@@ -12311,10 +12334,10 @@
         <v>1274</v>
       </c>
       <c r="I166" s="8" t="s">
+        <v>1430</v>
+      </c>
+      <c r="J166" s="9" t="s">
         <v>1431</v>
-      </c>
-      <c r="J166" s="9" t="s">
-        <v>1432</v>
       </c>
       <c r="K166" s="9">
         <v>34165</v>
@@ -12369,6 +12392,9 @@
       <c r="K167" s="10">
         <v>28415</v>
       </c>
+      <c r="L167" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="M167" s="10">
         <v>14486</v>
       </c>
@@ -12397,10 +12423,10 @@
         <v>1279</v>
       </c>
       <c r="I168" s="8" t="s">
+        <v>1427</v>
+      </c>
+      <c r="J168" s="9" t="s">
         <v>1428</v>
-      </c>
-      <c r="J168" s="9" t="s">
-        <v>1429</v>
       </c>
       <c r="K168" s="9">
         <v>33596</v>
@@ -12443,10 +12469,10 @@
         <v>1284</v>
       </c>
       <c r="I169" s="8" t="s">
+        <v>1425</v>
+      </c>
+      <c r="J169" s="9" t="s">
         <v>1426</v>
-      </c>
-      <c r="J169" s="9" t="s">
-        <v>1427</v>
       </c>
       <c r="K169" s="9">
         <v>32099</v>
@@ -12489,10 +12515,10 @@
         <v>1288</v>
       </c>
       <c r="I170" s="8" t="s">
+        <v>1407</v>
+      </c>
+      <c r="J170" s="9" t="s">
         <v>1408</v>
-      </c>
-      <c r="J170" s="9" t="s">
-        <v>1409</v>
       </c>
       <c r="K170" s="9">
         <v>16544</v>
@@ -12541,7 +12567,7 @@
         <v>201</v>
       </c>
       <c r="J171" s="8" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="K171" s="8" t="s">
         <v>1079</v>
@@ -12574,10 +12600,10 @@
         <v>1295</v>
       </c>
       <c r="I172" s="8" t="s">
+        <v>1409</v>
+      </c>
+      <c r="J172" s="9" t="s">
         <v>1410</v>
-      </c>
-      <c r="J172" s="9" t="s">
-        <v>1411</v>
       </c>
       <c r="K172" s="9">
         <v>19559</v>
@@ -12658,10 +12684,10 @@
         <v>1299</v>
       </c>
       <c r="I174" s="8" t="s">
+        <v>1415</v>
+      </c>
+      <c r="J174" s="8" t="s">
         <v>1416</v>
-      </c>
-      <c r="J174" s="8" t="s">
-        <v>1417</v>
       </c>
       <c r="K174" s="9">
         <v>27226</v>
@@ -12707,10 +12733,10 @@
         <v>1305</v>
       </c>
       <c r="I175" s="8" t="s">
+        <v>1405</v>
+      </c>
+      <c r="J175" s="9" t="s">
         <v>1406</v>
-      </c>
-      <c r="J175" s="9" t="s">
-        <v>1407</v>
       </c>
       <c r="K175" s="9">
         <v>16486</v>
@@ -12759,6 +12785,9 @@
       <c r="K176" s="10">
         <v>30028</v>
       </c>
+      <c r="L176" s="8" t="s">
+        <v>1460</v>
+      </c>
       <c r="M176" s="7"/>
       <c r="P176"/>
     </row>
@@ -12788,7 +12817,7 @@
         <v>897</v>
       </c>
       <c r="J177" s="9" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="K177" s="9">
         <v>30028</v>
@@ -12831,10 +12860,10 @@
         <v>1316</v>
       </c>
       <c r="I178" s="8" t="s">
+        <v>1418</v>
+      </c>
+      <c r="J178" s="9" t="s">
         <v>1419</v>
-      </c>
-      <c r="J178" s="9" t="s">
-        <v>1420</v>
       </c>
       <c r="K178" s="9">
         <v>29967</v>
@@ -12877,10 +12906,10 @@
         <v>1321</v>
       </c>
       <c r="I179" s="8" t="s">
+        <v>1420</v>
+      </c>
+      <c r="J179" s="8" t="s">
         <v>1421</v>
-      </c>
-      <c r="J179" s="8" t="s">
-        <v>1422</v>
       </c>
       <c r="K179" s="9">
         <v>30093</v>
@@ -12966,10 +12995,10 @@
         <v>1327</v>
       </c>
       <c r="I181" s="8" t="s">
+        <v>1411</v>
+      </c>
+      <c r="J181" s="8" t="s">
         <v>1412</v>
-      </c>
-      <c r="J181" s="8" t="s">
-        <v>1413</v>
       </c>
       <c r="K181" s="9">
         <v>20701</v>
@@ -13015,10 +13044,10 @@
         <v>1333</v>
       </c>
       <c r="I182" s="8" t="s">
+        <v>1413</v>
+      </c>
+      <c r="J182" s="8" t="s">
         <v>1414</v>
-      </c>
-      <c r="J182" s="8" t="s">
-        <v>1415</v>
       </c>
       <c r="K182" s="9">
         <v>23118</v>
@@ -13061,13 +13090,13 @@
         <v>1337</v>
       </c>
       <c r="I183" s="8" t="s">
+        <v>1422</v>
+      </c>
+      <c r="J183" s="8" t="s">
         <v>1423</v>
       </c>
-      <c r="J183" s="8" t="s">
-        <v>1424</v>
-      </c>
-      <c r="K183" s="8" t="s">
-        <v>1338</v>
+      <c r="K183" s="9">
+        <v>28094</v>
       </c>
       <c r="L183" s="8" t="s">
         <v>14</v>
@@ -13076,10 +13105,10 @@
         <v>15220</v>
       </c>
       <c r="N183" s="8" t="s">
+        <v>1338</v>
+      </c>
+      <c r="O183" s="8" t="s">
         <v>1339</v>
-      </c>
-      <c r="O183" s="8" t="s">
-        <v>1340</v>
       </c>
       <c r="Q183"/>
       <c r="R183"/>
@@ -14574,9 +14603,11 @@
     <hyperlink ref="I77" r:id="rId205"/>
     <hyperlink ref="I73" r:id="rId206"/>
     <hyperlink ref="I72" r:id="rId207"/>
+    <hyperlink ref="J124" r:id="rId208"/>
+    <hyperlink ref="I135" r:id="rId209"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId208"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId210"/>
 </worksheet>
 </file>
 
@@ -14621,191 +14652,191 @@
       </c>
     </row>
     <row r="34" spans="1:34" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="56"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="57"/>
+      <c r="O34" s="57"/>
+      <c r="P34" s="57"/>
+      <c r="Q34" s="57"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="57"/>
+      <c r="N36" s="57"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="57"/>
+      <c r="Q36" s="57"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
+      <c r="A37" s="57"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="57"/>
+      <c r="Q37" s="57"/>
     </row>
     <row r="38" spans="1:34" ht="183" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
-      <c r="Q38" s="57"/>
-      <c r="U38" s="58" t="s">
+      <c r="B38" s="58"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="58"/>
+      <c r="U38" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="V38" s="59"/>
-      <c r="W38" s="59"/>
-      <c r="X38" s="59"/>
-      <c r="Y38" s="59"/>
-      <c r="Z38" s="59"/>
-      <c r="AA38" s="59"/>
-      <c r="AB38" s="59"/>
-      <c r="AC38" s="59"/>
-      <c r="AD38" s="59"/>
-      <c r="AE38" s="59"/>
-      <c r="AF38" s="59"/>
-      <c r="AG38" s="59"/>
-      <c r="AH38" s="59"/>
+      <c r="V38" s="60"/>
+      <c r="W38" s="60"/>
+      <c r="X38" s="60"/>
+      <c r="Y38" s="60"/>
+      <c r="Z38" s="60"/>
+      <c r="AA38" s="60"/>
+      <c r="AB38" s="60"/>
+      <c r="AC38" s="60"/>
+      <c r="AD38" s="60"/>
+      <c r="AE38" s="60"/>
+      <c r="AF38" s="60"/>
+      <c r="AG38" s="60"/>
+      <c r="AH38" s="60"/>
     </row>
     <row r="39" spans="1:34" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="57" t="s">
+      <c r="A39" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="57"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="57"/>
-      <c r="K39" s="57"/>
-      <c r="L39" s="57"/>
-      <c r="M39" s="57"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="57"/>
-      <c r="P39" s="57"/>
-      <c r="Q39" s="57"/>
-      <c r="U39" s="59"/>
-      <c r="V39" s="59"/>
-      <c r="W39" s="59"/>
-      <c r="X39" s="59"/>
-      <c r="Y39" s="59"/>
-      <c r="Z39" s="59"/>
-      <c r="AA39" s="59"/>
-      <c r="AB39" s="59"/>
-      <c r="AC39" s="59"/>
-      <c r="AD39" s="59"/>
-      <c r="AE39" s="59"/>
-      <c r="AF39" s="59"/>
-      <c r="AG39" s="59"/>
-      <c r="AH39" s="59"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="58"/>
+      <c r="J39" s="58"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="58"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="58"/>
+      <c r="U39" s="60"/>
+      <c r="V39" s="60"/>
+      <c r="W39" s="60"/>
+      <c r="X39" s="60"/>
+      <c r="Y39" s="60"/>
+      <c r="Z39" s="60"/>
+      <c r="AA39" s="60"/>
+      <c r="AB39" s="60"/>
+      <c r="AC39" s="60"/>
+      <c r="AD39" s="60"/>
+      <c r="AE39" s="60"/>
+      <c r="AF39" s="60"/>
+      <c r="AG39" s="60"/>
+      <c r="AH39" s="60"/>
     </row>
     <row r="40" spans="1:34" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="57"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="57"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="57"/>
-      <c r="M40" s="57"/>
-      <c r="N40" s="57"/>
-      <c r="O40" s="57"/>
-      <c r="P40" s="57"/>
-      <c r="Q40" s="57"/>
-      <c r="U40" s="59"/>
-      <c r="V40" s="59"/>
-      <c r="W40" s="59"/>
-      <c r="X40" s="59"/>
-      <c r="Y40" s="59"/>
-      <c r="Z40" s="59"/>
-      <c r="AA40" s="59"/>
-      <c r="AB40" s="59"/>
-      <c r="AC40" s="59"/>
-      <c r="AD40" s="59"/>
-      <c r="AE40" s="59"/>
-      <c r="AF40" s="59"/>
-      <c r="AG40" s="59"/>
-      <c r="AH40" s="59"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="58"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="58"/>
+      <c r="U40" s="60"/>
+      <c r="V40" s="60"/>
+      <c r="W40" s="60"/>
+      <c r="X40" s="60"/>
+      <c r="Y40" s="60"/>
+      <c r="Z40" s="60"/>
+      <c r="AA40" s="60"/>
+      <c r="AB40" s="60"/>
+      <c r="AC40" s="60"/>
+      <c r="AD40" s="60"/>
+      <c r="AE40" s="60"/>
+      <c r="AF40" s="60"/>
+      <c r="AG40" s="60"/>
+      <c r="AH40" s="60"/>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56"/>
-      <c r="K41" s="56"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
-      <c r="O41" s="56"/>
-      <c r="P41" s="56"/>
-      <c r="Q41" s="56"/>
+      <c r="A41" s="57"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="57"/>
+      <c r="N41" s="57"/>
+      <c r="O41" s="57"/>
+      <c r="P41" s="57"/>
+      <c r="Q41" s="57"/>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -14968,14 +14999,14 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
       <c r="G14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>

</xml_diff>